<commit_message>
Fixing PDF display and modifying csv sample data
</commit_message>
<xml_diff>
--- a/backend/database_functions/PaRx Sample Data - Copy.xlsx
+++ b/backend/database_functions/PaRx Sample Data - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\VS Code\C01 Projects\c01w24-project-RxValidators\backend\database_functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E73E113-368D-476B-BE7A-330058C2E98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488ADD01-764F-4754-B399-30D60F47F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{67FA1224-4162-4CC1-B293-B63621348A26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -467,7 +467,7 @@
   <dimension ref="A1:F108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,11 +560,44 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>4426</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>4426</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="3"/>
@@ -963,15 +996,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010002094DA39EF1414CAD215C7869284230" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="65c042d0f250bfa93de76601d4f10e11">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c70aaa4c-9d63-4e79-8dfc-29a3224cd5eb" xmlns:ns3="a304d97d-8119-45dd-9f65-302c8967cb1f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="296f89f1b3b9fff402353141abdeed73" ns2:_="" ns3:_="">
     <xsd:import namespace="c70aaa4c-9d63-4e79-8dfc-29a3224cd5eb"/>
@@ -1220,15 +1244,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4830F3C7-40C7-4D54-A60E-39E24E2BC772}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{009D7525-7CB1-4939-80B1-FB73B5886437}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1245,4 +1270,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4830F3C7-40C7-4D54-A60E-39E24E2BC772}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>